<commit_message>
fix data entry errors in codestamps
</commit_message>
<xml_diff>
--- a/data-raw/res2C_focus.xlsx
+++ b/data-raw/res2C_focus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zurp/Dropbox (Personal)/diss/analy/vid-coding/res2C-focus. in prog/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21C76D00-C44F-5F4C-AF78-6598AE8EE338}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F7C083-A0F5-F041-A516-F85F40A3E558}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="10000" windowHeight="17540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,9 +91,6 @@
     <t>05:37</t>
   </si>
   <si>
-    <t>05:58</t>
-  </si>
-  <si>
     <t>05:44</t>
   </si>
   <si>
@@ -407,6 +404,9 @@
   </si>
   <si>
     <t>16:35</t>
+  </si>
+  <si>
+    <t>05:38</t>
   </si>
 </sst>
 </file>
@@ -1012,8 +1012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DE10D47-70A0-574D-B2E3-ED3263117924}">
   <dimension ref="A1:F132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1143,7 +1143,7 @@
         <v>19</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -1158,10 +1158,10 @@
         <v>17</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>20</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>21</v>
       </c>
       <c r="F8" s="1"/>
     </row>
@@ -1176,10 +1176,10 @@
         <v>17</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>22</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>23</v>
       </c>
       <c r="F9" s="1"/>
     </row>
@@ -1194,10 +1194,10 @@
         <v>17</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>24</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -1212,10 +1212,10 @@
         <v>17</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>26</v>
       </c>
       <c r="F11" s="1"/>
     </row>
@@ -1230,10 +1230,10 @@
         <v>17</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>27</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>28</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -1245,13 +1245,13 @@
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>30</v>
       </c>
       <c r="F13" s="1"/>
     </row>
@@ -1266,10 +1266,10 @@
         <v>17</v>
       </c>
       <c r="D14" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>30</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>31</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -1284,10 +1284,10 @@
         <v>17</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>33</v>
       </c>
       <c r="F15" s="1"/>
     </row>
@@ -1299,13 +1299,13 @@
         <v>7</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>35</v>
       </c>
       <c r="F16" s="1"/>
     </row>
@@ -1320,10 +1320,10 @@
         <v>15</v>
       </c>
       <c r="D17" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>36</v>
       </c>
       <c r="F17" s="1"/>
     </row>
@@ -1335,13 +1335,13 @@
         <v>7</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>37</v>
       </c>
       <c r="F18" s="1"/>
     </row>
@@ -1353,13 +1353,13 @@
         <v>7</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="F19" s="1"/>
     </row>
@@ -1371,13 +1371,13 @@
         <v>7</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D20" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="F20" s="1"/>
     </row>
@@ -1392,10 +1392,10 @@
         <v>15</v>
       </c>
       <c r="D21" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>41</v>
       </c>
       <c r="F21" s="1"/>
     </row>
@@ -1407,13 +1407,13 @@
         <v>7</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="E22" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="F22" s="1"/>
     </row>
@@ -1425,13 +1425,13 @@
         <v>13</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D23" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="E23" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="F23" s="1"/>
     </row>
@@ -1446,10 +1446,10 @@
         <v>15</v>
       </c>
       <c r="D24" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="F24" s="1"/>
     </row>
@@ -1464,10 +1464,10 @@
         <v>11</v>
       </c>
       <c r="D25" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="F25" s="1"/>
     </row>
@@ -1482,10 +1482,10 @@
         <v>15</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="F26" s="1"/>
     </row>
@@ -1500,10 +1500,10 @@
         <v>11</v>
       </c>
       <c r="D27" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="E27" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="F27" s="1"/>
     </row>
@@ -1518,10 +1518,10 @@
         <v>15</v>
       </c>
       <c r="D28" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="F28" s="1"/>
     </row>
@@ -1536,10 +1536,10 @@
         <v>15</v>
       </c>
       <c r="D29" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="F29" s="1"/>
     </row>
@@ -1554,10 +1554,10 @@
         <v>17</v>
       </c>
       <c r="D30" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="F30" s="1"/>
     </row>
@@ -1572,10 +1572,10 @@
         <v>17</v>
       </c>
       <c r="D31" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="F31" s="1"/>
     </row>
@@ -1590,10 +1590,10 @@
         <v>17</v>
       </c>
       <c r="D32" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>54</v>
       </c>
       <c r="F32" s="1"/>
     </row>
@@ -1608,10 +1608,10 @@
         <v>17</v>
       </c>
       <c r="D33" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E33" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="E33" s="3" t="s">
-        <v>56</v>
       </c>
       <c r="F33" s="1"/>
     </row>
@@ -1626,10 +1626,10 @@
         <v>17</v>
       </c>
       <c r="D34" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E34" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="F34" s="1"/>
     </row>
@@ -1644,10 +1644,10 @@
         <v>11</v>
       </c>
       <c r="D35" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="E35" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>59</v>
       </c>
       <c r="F35" s="1"/>
     </row>
@@ -1662,10 +1662,10 @@
         <v>15</v>
       </c>
       <c r="D36" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E36" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>60</v>
       </c>
       <c r="F36" s="1"/>
     </row>
@@ -1680,10 +1680,10 @@
         <v>15</v>
       </c>
       <c r="D37" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="F37" s="1"/>
     </row>
@@ -1698,10 +1698,10 @@
         <v>15</v>
       </c>
       <c r="D38" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="E38" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="F38" s="1"/>
     </row>
@@ -1716,10 +1716,10 @@
         <v>8</v>
       </c>
       <c r="D39" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E39" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="E39" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="F39" s="1"/>
     </row>
@@ -1734,10 +1734,10 @@
         <v>11</v>
       </c>
       <c r="D40" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E40" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="E40" s="3" t="s">
-        <v>69</v>
       </c>
       <c r="F40" s="1"/>
     </row>
@@ -1752,10 +1752,10 @@
         <v>15</v>
       </c>
       <c r="D41" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>71</v>
       </c>
       <c r="F41" s="1"/>
     </row>
@@ -1770,10 +1770,10 @@
         <v>15</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>20</v>
+        <v>125</v>
       </c>
       <c r="F42" s="1"/>
     </row>
@@ -1788,10 +1788,10 @@
         <v>15</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>20</v>
+        <v>125</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F43" s="3"/>
     </row>
@@ -1806,10 +1806,10 @@
         <v>11</v>
       </c>
       <c r="D44" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E44" s="3" t="s">
         <v>73</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>74</v>
       </c>
       <c r="F44" s="3"/>
     </row>
@@ -1824,10 +1824,10 @@
         <v>15</v>
       </c>
       <c r="D45" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E45" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="E45" s="3" t="s">
-        <v>76</v>
       </c>
       <c r="F45" s="3"/>
     </row>
@@ -1842,10 +1842,10 @@
         <v>11</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1859,10 +1859,10 @@
         <v>15</v>
       </c>
       <c r="D47" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47" s="3" t="s">
         <v>78</v>
-      </c>
-      <c r="E47" s="3" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1876,10 +1876,10 @@
         <v>15</v>
       </c>
       <c r="D48" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="E48" s="3" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1893,10 +1893,10 @@
         <v>15</v>
       </c>
       <c r="D49" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>82</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1910,10 +1910,10 @@
         <v>15</v>
       </c>
       <c r="D50" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E50" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1927,10 +1927,10 @@
         <v>11</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1944,10 +1944,10 @@
         <v>11</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1961,10 +1961,10 @@
         <v>15</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1978,10 +1978,10 @@
         <v>17</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1995,10 +1995,10 @@
         <v>15</v>
       </c>
       <c r="D55" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E55" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="E55" s="3" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -2012,10 +2012,10 @@
         <v>15</v>
       </c>
       <c r="D56" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E56" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="E56" s="3" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -2029,10 +2029,10 @@
         <v>15</v>
       </c>
       <c r="D57" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="E57" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="E57" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2046,10 +2046,10 @@
         <v>15</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2063,10 +2063,10 @@
         <v>15</v>
       </c>
       <c r="D59" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="E59" s="3" t="s">
         <v>97</v>
-      </c>
-      <c r="E59" s="3" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2080,10 +2080,10 @@
         <v>11</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E60" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2097,10 +2097,10 @@
         <v>15</v>
       </c>
       <c r="D61" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E61" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2114,10 +2114,10 @@
         <v>17</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2131,10 +2131,10 @@
         <v>17</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2689,7 +2689,7 @@
         <v>12</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -2704,10 +2704,10 @@
         <v>17</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -2722,7 +2722,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>19</v>
@@ -2743,7 +2743,7 @@
         <v>19</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -2758,10 +2758,10 @@
         <v>15</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -2776,10 +2776,10 @@
         <v>11</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F8" s="1"/>
     </row>
@@ -2794,10 +2794,10 @@
         <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F9" s="1"/>
     </row>
@@ -2812,10 +2812,10 @@
         <v>15</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -2830,10 +2830,10 @@
         <v>11</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>109</v>
       </c>
       <c r="F11" s="1"/>
     </row>
@@ -2845,13 +2845,13 @@
         <v>7</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>111</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -2866,10 +2866,10 @@
         <v>15</v>
       </c>
       <c r="D13" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>111</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="F13" s="1"/>
     </row>
@@ -2881,13 +2881,13 @@
         <v>7</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -2902,10 +2902,10 @@
         <v>15</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F15" s="1"/>
     </row>
@@ -2920,10 +2920,10 @@
         <v>15</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>114</v>
       </c>
       <c r="F16" s="1"/>
     </row>
@@ -2938,10 +2938,10 @@
         <v>15</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F17" s="1"/>
     </row>
@@ -2956,10 +2956,10 @@
         <v>17</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F18" s="1"/>
     </row>
@@ -2974,10 +2974,10 @@
         <v>17</v>
       </c>
       <c r="D19" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E19" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>116</v>
       </c>
       <c r="F19" s="1"/>
     </row>
@@ -2992,10 +2992,10 @@
         <v>17</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F20" s="1"/>
     </row>
@@ -3010,10 +3010,10 @@
         <v>15</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F21" s="1"/>
     </row>
@@ -3028,10 +3028,10 @@
         <v>15</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F22" s="1"/>
     </row>
@@ -3046,10 +3046,10 @@
         <v>15</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F23" s="1"/>
     </row>
@@ -3064,10 +3064,10 @@
         <v>17</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F24" s="1"/>
     </row>
@@ -3082,10 +3082,10 @@
         <v>17</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F25" s="1"/>
     </row>
@@ -3100,10 +3100,10 @@
         <v>8</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F26" s="1"/>
     </row>
@@ -3118,10 +3118,10 @@
         <v>17</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F27" s="1"/>
     </row>
@@ -3136,10 +3136,10 @@
         <v>17</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F28" s="1"/>
     </row>
@@ -3154,10 +3154,10 @@
         <v>17</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F29" s="1"/>
     </row>
@@ -3172,10 +3172,10 @@
         <v>11</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F30" s="1"/>
     </row>
@@ -3190,10 +3190,10 @@
         <v>15</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="F31" s="1"/>
     </row>
@@ -3208,10 +3208,10 @@
         <v>15</v>
       </c>
       <c r="D32" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>116</v>
       </c>
       <c r="F32" s="1"/>
     </row>
@@ -3226,10 +3226,10 @@
         <v>15</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F33" s="1"/>
     </row>

</xml_diff>